<commit_message>
Low Resolution validated and updated Demo
</commit_message>
<xml_diff>
--- a/Demo/C13_succ_corr.xlsx
+++ b/Demo/C13_succ_corr.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raaisa/Documents/NA_Correction/Demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{59A0CFAC-5806-4641-88C4-55980E8F12DE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E445503-556D-0045-901A-2BC065804694}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15440" activeTab="1"/>
+    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="C13_succ_corr" sheetId="1" r:id="rId1"/>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -947,7 +947,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1032,7 +1032,7 @@
         <v>1.0005502718446599</v>
       </c>
       <c r="M2">
-        <v>0.60196644231571805</v>
+        <v>0.60231416460095</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -1073,7 +1073,7 @@
         <v>1.0005502718446599</v>
       </c>
       <c r="M3">
-        <v>0.20123561899214301</v>
+        <v>0.20099431282114799</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -1114,7 +1114,7 @@
         <v>1.0005502718446599</v>
       </c>
       <c r="M4">
-        <v>0.11518784505773701</v>
+        <v>0.115131121340268</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -1155,7 +1155,7 @@
         <v>1.0005502718446599</v>
       </c>
       <c r="M5">
-        <v>5.0966149946432303E-2</v>
+        <v>5.0928167309775001E-2</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -1196,7 +1196,7 @@
         <v>1.0005502718446599</v>
       </c>
       <c r="M6">
-        <v>3.0643943687967998E-2</v>
+        <v>3.0632233927857501E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1205,7 +1205,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -1214,7 +1214,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -1239,7 +1241,7 @@
         <v>0.60206999999999999</v>
       </c>
       <c r="D2">
-        <v>0.60196644231571805</v>
+        <v>0.60265920170656095</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1253,7 +1255,7 @@
         <v>0.20118</v>
       </c>
       <c r="D3">
-        <v>0.20123561899214301</v>
+        <v>0.201109452892586</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1267,7 +1269,7 @@
         <v>0.11516999999999999</v>
       </c>
       <c r="D4">
-        <v>0.11518784505773701</v>
+        <v>0.115197074477696</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1281,7 +1283,7 @@
         <v>5.0950000000000002E-2</v>
       </c>
       <c r="D5">
-        <v>5.0966149946432303E-2</v>
+        <v>5.0957341631873598E-2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1295,7 +1297,7 @@
         <v>3.0640000000000001E-2</v>
       </c>
       <c r="D6">
-        <v>3.0643943687967998E-2</v>
+        <v>3.06497816761158E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Demo files validated after changes
</commit_message>
<xml_diff>
--- a/Demo/C13_succ_corr.xlsx
+++ b/Demo/C13_succ_corr.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raaisa/Documents/NA_Correction/Demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E445503-556D-0045-901A-2BC065804694}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C11E093-72A7-0B4A-8DC5-8E7A8D1A0E3F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12200" yWindow="1280" windowWidth="27640" windowHeight="15440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="C13_succ_corr" sheetId="1" r:id="rId1"/>

</xml_diff>